<commit_message>
client res export use pb encode
</commit_message>
<xml_diff>
--- a/resExport/xlsx/test.xlsx
+++ b/resExport/xlsx/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -25,6 +25,18 @@
   </si>
   <si>
     <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaaaa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbbbb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -371,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +401,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -400,8 +415,11 @@
       <c r="C2">
         <v>100</v>
       </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,6 +428,9 @@
       </c>
       <c r="C3">
         <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>